<commit_message>
Fixed sheetName trailing space in frontend
</commit_message>
<xml_diff>
--- a/Group A/SAMPLE.xlsx
+++ b/Group A/SAMPLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ender\Desktop\Accounting project\Group A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C69C3A6-ECD4-4DBA-BED2-DFE727D5321C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5369BE7B-253D-45E8-B2BC-63FB3E7B21BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" firstSheet="1" xr2:uid="{45CB8D84-C63B-4155-8EA6-2EF36D73B191}"/>
+    <workbookView xWindow="6540" yWindow="2112" windowWidth="17280" windowHeight="8880" xr2:uid="{45CB8D84-C63B-4155-8EA6-2EF36D73B191}"/>
   </bookViews>
   <sheets>
     <sheet name="CHARTS OF ACCOUNTS " sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
   <si>
     <r>
       <t>1. March 1, 2025</t>
@@ -605,6 +605,9 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Testerino</t>
   </si>
 </sst>
 </file>
@@ -2418,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62133890-CC46-4EEC-8C5A-E99A2C83F793}">
   <dimension ref="A2:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2587,6 +2590,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
       <c r="G13" s="13"/>
     </row>
     <row r="17" spans="6:11" x14ac:dyDescent="0.3">

</xml_diff>